<commit_message>
V0.01 - 4 update
</commit_message>
<xml_diff>
--- a/Konzept (20.03.2023)/MappeShips.xlsx
+++ b/Konzept (20.03.2023)/MappeShips.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae64ddbbd6707e46/Desktop/gitHub/AutoBattlerSW/Konzept (20.03.2023)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathiasalexander.pal\OneDrive - CGM\Desktop\EclipsePortable\Data\workspace\AutoBattlerSW\Konzept (20.03.2023)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="296" documentId="14_{8A0C77D5-7AFE-4DE9-891A-EAB549D89894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DA4B1E5-0A71-4CF3-880E-A46F16B6FC46}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FCB636-1C91-4C45-B3D5-C1AB5610A0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{791FD962-70B8-4E21-813D-7E34BE83B7C2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{791FD962-70B8-4E21-813D-7E34BE83B7C2}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -357,13 +357,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -392,10 +391,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -838,30 +833,30 @@
   <dimension ref="B3:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -908,7 +903,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -956,7 +951,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>19</v>
       </c>
@@ -999,12 +994,12 @@
         <f>SUM(Tabelle10[[#This Row],[all ship HP]:[all ship shield]])</f>
         <v>17700</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="Q6">
         <f>SUM(Tabelle13[credit cost])</f>
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>20</v>
       </c>
@@ -1047,12 +1042,12 @@
         <f>SUM(Tabelle10[[#This Row],[all ship HP]:[all ship shield]])</f>
         <v>19200</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="Q7">
         <f>SUM(Tabelle134[credit cost])</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -1087,9 +1082,8 @@
         <f>SUM(Tabelle10[[#This Row],[all ship HP]:[all ship shield]])</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -1121,9 +1115,8 @@
         <f>SUM(Tabelle10[[#This Row],[all ship HP]:[all ship shield]])</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="3"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -1152,7 +1145,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -1182,7 +1175,7 @@
       </c>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -1211,12 +1204,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>1</v>
       </c>
@@ -1248,7 +1241,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>28</v>
       </c>
@@ -1277,7 +1270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>29</v>
       </c>
@@ -1306,7 +1299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>30</v>
       </c>
@@ -1335,7 +1328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>31</v>
       </c>
@@ -1364,7 +1357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>32</v>
       </c>
@@ -1393,7 +1386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -1422,7 +1415,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>22</v>
       </c>
@@ -1451,7 +1444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>34</v>
       </c>
@@ -1480,7 +1473,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>33</v>
       </c>
@@ -1509,12 +1502,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>1</v>
       </c>
@@ -1546,7 +1539,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>35</v>
       </c>
@@ -1575,7 +1568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>36</v>
       </c>
@@ -1604,7 +1597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>37</v>
       </c>
@@ -1633,7 +1626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>38</v>
       </c>
@@ -1662,7 +1655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>44</v>
       </c>
@@ -1688,10 +1681,10 @@
         <v>51</v>
       </c>
       <c r="K32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>39</v>
       </c>
@@ -1720,7 +1713,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>41</v>
       </c>
@@ -1746,10 +1739,10 @@
         <v>51</v>
       </c>
       <c r="K34">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>40</v>
       </c>
@@ -1775,10 +1768,10 @@
         <v>51</v>
       </c>
       <c r="K35">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>42</v>
       </c>
@@ -1807,7 +1800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>43</v>
       </c>
@@ -1839,6 +1832,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;9&amp;K000000 Internal Use Only</oddFooter>
+  </headerFooter>
   <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -1898,21 +1894,21 @@
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -1935,7 +1931,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>58</v>
       </c>
@@ -1959,7 +1955,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>57</v>
       </c>
@@ -1983,7 +1979,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>56</v>
       </c>
@@ -2007,7 +2003,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>55</v>
       </c>
@@ -2031,7 +2027,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>54</v>
       </c>
@@ -2052,30 +2048,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="G10" t="e" cm="1">
         <f t="array" ref="G10">_xlfn.IFS(D10 = "none", "0", D10 = "shield", "2", D10 = "hp", "2", D10 = "all", "3"  )</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="G11" t="e" cm="1">
         <f t="array" ref="G11">_xlfn.IFS(D11 = "none", "0", D11 = "shield", "2", D11 = "hp", "2", D11 = "all", "3"  )</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="G12" t="e" cm="1">
         <f t="array" ref="G12">_xlfn.IFS(D12 = "none", "0", D12 = "shield", "2", D12 = "hp", "2", D12 = "all", "3"  )</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>46</v>
       </c>
@@ -2095,7 +2091,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>51</v>
       </c>
@@ -2104,7 +2100,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>76</v>
       </c>
@@ -2119,7 +2115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>75</v>
       </c>
@@ -2134,7 +2130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>77</v>
       </c>
@@ -2149,25 +2145,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G22" t="e" cm="1">
         <f t="array" ref="G22">_xlfn.IFS(D22 = "none", "0", D22 = "shield", "2", D22 = "hp", "2", D22 = "all", "3"  )</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G23" t="e" cm="1">
         <f t="array" ref="G23">_xlfn.IFS(D23 = "none", "0", D23 = "shield", "2", D23 = "hp", "2", D23 = "all", "3"  )</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G24" t="e" cm="1">
         <f t="array" ref="G24">_xlfn.IFS(D24 = "none", "0", D24 = "shield", "2", D24 = "hp", "2", D24 = "all", "3"  )</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G25" t="e" cm="1">
         <f t="array" ref="G25">_xlfn.IFS(D25 = "none", "0", D25 = "shield", "2", D25 = "hp", "2", D25 = "all", "3"  )</f>
         <v>#N/A</v>
@@ -2180,6 +2176,9 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;9&amp;K000000 Internal Use Only</oddFooter>
+  </headerFooter>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
@@ -2195,17 +2194,17 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>46</v>
       </c>
@@ -2227,6 +2226,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;9&amp;K000000 Internal Use Only</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2241,12 +2243,12 @@
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -2257,7 +2259,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>51</v>
       </c>
@@ -2268,7 +2270,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -2279,7 +2281,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -2290,7 +2292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -2301,15 +2303,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;9&amp;K000000 Internal Use Only</oddFooter>
+  </headerFooter>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{fbf47bbe-a0a2-4c04-9ba4-22f94012202d}" enabled="1" method="Standard" siteId="{69602cf4-a76e-4265-955f-03c329c50608}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>